<commit_message>
Updates to PROVIDE ontology templates
</commit_message>
<xml_diff>
--- a/Load/ontology/Gates/PROVIDE/doc/PROVIDE_non-raw_detection_template.xlsx
+++ b/Load/ontology/Gates/PROVIDE/doc/PROVIDE_non-raw_detection_template.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sshahsimpson/Documents/Git/ApiCommonData/Load/ontology/Gates/PROVIDE/doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CD700A-A328-BF45-8CBE-9B4F0E415A8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56260651-E965-E74A-8752-F99D050DE3B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1080" windowWidth="33600" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="460" windowWidth="23460" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="raw_detection_template" sheetId="1" r:id="rId1"/>
+    <sheet name="non-raw_detection_template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="94">
   <si>
     <t>variable</t>
   </si>
@@ -70,9 +70,6 @@
     <t>E.g.: blood, stool, urine</t>
   </si>
   <si>
-    <t>urine</t>
-  </si>
-  <si>
     <t>Norovirus</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
   </si>
   <si>
     <t>enterotoxic or virulence factor tested negative</t>
-  </si>
-  <si>
-    <t>blood</t>
   </si>
   <si>
     <t>Parent term in ClinEpi</t>
@@ -277,6 +271,60 @@
   </si>
   <si>
     <t>ELISA</t>
+  </si>
+  <si>
+    <t>Ancylostomatidae</t>
+  </si>
+  <si>
+    <t>ext_lab_bv_polcul::polioc</t>
+  </si>
+  <si>
+    <t>culture</t>
+  </si>
+  <si>
+    <t>Enterovirus</t>
+  </si>
+  <si>
+    <t>Poliovirus</t>
+  </si>
+  <si>
+    <t>ext_lab_bv_polpcr::sabin</t>
+  </si>
+  <si>
+    <t>ext_lab_bv_polpcr::ns_othr</t>
+  </si>
+  <si>
+    <t>rRT-PCR</t>
+  </si>
+  <si>
+    <t>Poliovirus vaccine serotype</t>
+  </si>
+  <si>
+    <t>Poliovirus non-vaccine serotype</t>
+  </si>
+  <si>
+    <t>ext_lab_bv_qpcr::s1</t>
+  </si>
+  <si>
+    <t>ext_lab_bv_qpcr::s2</t>
+  </si>
+  <si>
+    <t>ext_lab_bv_qpcr::s3</t>
+  </si>
+  <si>
+    <t>multiplexed qRT-PCR</t>
+  </si>
+  <si>
+    <t>Poliovirus serotype Sabin 1</t>
+  </si>
+  <si>
+    <t>Poliovirus serotype Sabin 2</t>
+  </si>
+  <si>
+    <t>Poliovirus serotype Sabin 3</t>
+  </si>
+  <si>
+    <t>ext_mgmt_bv_ddep::rotads</t>
   </si>
 </sst>
 </file>
@@ -774,7 +822,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -783,6 +831,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1138,13 +1187,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D28" sqref="D28"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,16 +1236,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>9</v>
@@ -1208,7 +1257,7 @@
         <v>10</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -1216,7 +1265,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>8</v>
@@ -1225,33 +1274,33 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="125" customHeight="1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M3" s="5" t="str">
         <f t="shared" ref="M3:M12" si="0">TRIM(IF($F3="",$E3,"")
@@ -1265,32 +1314,32 @@
         <v>10a. Micro Eh/Ed, by microscopy</v>
       </c>
       <c r="N3" s="2" t="str">
-        <f t="shared" ref="N3:N22" si="1">TRIM($D3&amp;" in "&amp;$B3)</f>
+        <f t="shared" ref="N3:N29" si="1">TRIM($E3&amp;" in "&amp;$B3)</f>
+        <v>in stool</v>
+      </c>
+      <c r="O3" s="2" t="str">
+        <f>TRIM($D3&amp;" in "&amp;$B3)</f>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O3" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B3)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M4" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1298,31 +1347,31 @@
       </c>
       <c r="N4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Bacteria in blood</v>
-      </c>
-      <c r="O4" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B4)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>Escherichia in stool</v>
+      </c>
+      <c r="O4" s="2" t="str">
+        <f t="shared" ref="O4:O29" si="2">TRIM($D4&amp;" in "&amp;$B4)</f>
+        <v>Bacteria in stool</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="M5" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1330,31 +1379,31 @@
       </c>
       <c r="N5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Eukaryota in urine</v>
-      </c>
-      <c r="O5" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B5)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+        <v>Endolimax in stool</v>
+      </c>
+      <c r="O5" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Eukaryota in stool</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M6" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1362,31 +1411,31 @@
       </c>
       <c r="N6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>Eukaryota in urine</v>
-      </c>
-      <c r="O6" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B6)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>Iodamoeba in stool</v>
+      </c>
+      <c r="O6" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Eukaryota in stool</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M7" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1394,31 +1443,31 @@
       </c>
       <c r="N7" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Blastocystis in stool</v>
+      </c>
+      <c r="O7" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O7" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B7)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M8" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1426,31 +1475,31 @@
       </c>
       <c r="N8" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Trichomonas in stool</v>
+      </c>
+      <c r="O8" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O8" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B8)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M9" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1458,31 +1507,31 @@
       </c>
       <c r="N9" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Giardia in stool</v>
+      </c>
+      <c r="O9" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O9" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B9)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M10" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1490,31 +1539,31 @@
       </c>
       <c r="N10" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Ascaris in stool</v>
+      </c>
+      <c r="O10" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O10" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B10)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M11" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1522,28 +1571,31 @@
       </c>
       <c r="N11" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Trichuris in stool</v>
+      </c>
+      <c r="O11" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O11" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B11)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="E12" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="F12" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M12" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1551,34 +1603,34 @@
       </c>
       <c r="N12" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Ancylostomatidae in stool</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O12" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B12)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="M13" s="5" t="str">
-        <f t="shared" ref="M13:M22" si="2">TRIM(IF($F13="",$E13,"")
+        <f t="shared" ref="M13:M29" si="3">TRIM(IF($F13="",$E13,"")
 &amp;IF($F13&lt;&gt;"",$F13,"")
 &amp;IF($H13&lt;&gt;""," "&amp;$H13,"")
 &amp;IF(OR($H13="LT",$H13="ST",$H13&lt;&gt;""),"-pos","")
@@ -1590,324 +1642,524 @@
       </c>
       <c r="N13" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Hymenolepis in stool</v>
+      </c>
+      <c r="O13" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O13" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B13)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M14" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Strongyloides stercoralis, by microscopy</v>
       </c>
       <c r="N14" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Strongyloides in stool</v>
+      </c>
+      <c r="O14" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O14" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B14)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M15" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Rotavirus, by qPCR</v>
       </c>
       <c r="N15" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Rotavirus in stool</v>
+      </c>
+      <c r="O15" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Virus in stool</v>
       </c>
-      <c r="O15" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B15)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="M16" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Astrovirus, by qPCR</v>
       </c>
       <c r="N16" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Astrovirus in stool</v>
+      </c>
+      <c r="O16" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Virus in stool</v>
       </c>
-      <c r="O16" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B16)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M17" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Norovirus, by qPCR</v>
       </c>
       <c r="N17" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Norovirus in stool</v>
+      </c>
+      <c r="O17" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Virus in stool</v>
       </c>
-      <c r="O17" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B17)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M18" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Sapovirus, by qPCR</v>
       </c>
       <c r="N18" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Sapovirus in stool</v>
+      </c>
+      <c r="O18" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Virus in stool</v>
       </c>
-      <c r="O18" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B18)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="M19" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Giardia, by qPCR</v>
       </c>
       <c r="N19" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Giardia in stool</v>
+      </c>
+      <c r="O19" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O19" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B19)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M20" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Entamoeba histolytica, by qPCR</v>
       </c>
       <c r="N20" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Entamoeba in stool</v>
+      </c>
+      <c r="O20" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O20" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B20)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M21" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Cryptosporidium, by qPCR</v>
       </c>
       <c r="N21" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Cryptosporidium in stool</v>
+      </c>
+      <c r="O21" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Eukaryota in stool</v>
       </c>
-      <c r="O21" s="2" t="e">
-        <f>TRIM(#REF!&amp;" in "&amp;$B21)</f>
-        <v>#REF!</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M22" s="5" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Rotavirus, by ELISA</v>
       </c>
       <c r="N22" s="2" t="str">
         <f t="shared" si="1"/>
+        <v>Rotavirus in stool</v>
+      </c>
+      <c r="O22" s="2" t="str">
+        <f t="shared" si="2"/>
         <v>Virus in stool</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24"/>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25"/>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29"/>
-      <c r="F29" s="3"/>
+    <row r="23" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M23" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Poliovirus, by culture</v>
+      </c>
+      <c r="N23" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Enterovirus in stool</v>
+      </c>
+      <c r="O23" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Virus in stool</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="M24" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Poliovirus vaccine serotype, by rRT-PCR</v>
+      </c>
+      <c r="N24" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Enterovirus in stool</v>
+      </c>
+      <c r="O24" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Virus in stool</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="M25" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Poliovirus non-vaccine serotype, by rRT-PCR</v>
+      </c>
+      <c r="N25" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Enterovirus in stool</v>
+      </c>
+      <c r="O25" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Virus in stool</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" t="s">
+        <v>90</v>
+      </c>
+      <c r="M26" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Poliovirus serotype Sabin 1, by multiplexed qRT-PCR</v>
+      </c>
+      <c r="N26" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Enterovirus in stool</v>
+      </c>
+      <c r="O26" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Virus in stool</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" t="s">
+        <v>91</v>
+      </c>
+      <c r="M27" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Poliovirus serotype Sabin 2, by multiplexed qRT-PCR</v>
+      </c>
+      <c r="N27" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Enterovirus in stool</v>
+      </c>
+      <c r="O27" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Virus in stool</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F28" t="s">
+        <v>92</v>
+      </c>
+      <c r="M28" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Poliovirus serotype Sabin 3, by multiplexed qRT-PCR</v>
+      </c>
+      <c r="N28" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Enterovirus in stool</v>
+      </c>
+      <c r="O28" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Virus in stool</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="M29" s="5" t="str">
+        <f t="shared" si="3"/>
+        <v>Rotavirus, by ELISA</v>
+      </c>
+      <c r="N29" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Rotavirus in stool</v>
+      </c>
+      <c r="O29" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Virus in stool</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30"/>
@@ -2052,18 +2304,6 @@
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65"/>
       <c r="F65" s="3"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66"/>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67"/>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68"/>
-      <c r="F68" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>